<commit_message>
PCIC climate normal departures (appendix)
</commit_message>
<xml_diff>
--- a/R-inputs_UBC-forWater-MSc_HMc/tables/Workbooks/weather_anomaly_PCIC.xlsx
+++ b/R-inputs_UBC-forWater-MSc_HMc/tables/Workbooks/weather_anomaly_PCIC.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Documents\UBC_MSc\Thesis_UBC-forWater-MSc_HMc\R_UBC_MSc_thesis\R-inputs_UBC-forWater-MSc_HMc\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\2020_Thesis_gitdocs\UBC_MSc_thesis\R-inputs_UBC-forWater-MSc_HMc\tables\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21934E29-C9F9-40FC-8D61-A5A992AFA0E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{316E0485-2B27-411B-8A0B-09670945CE8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="795" windowWidth="18780" windowHeight="14415" xr2:uid="{7680C772-8F90-439C-BDD5-995D84FBCB52}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7680C772-8F90-439C-BDD5-995D84FBCB52}"/>
   </bookViews>
   <sheets>
     <sheet name="weather_anomaly_PCIC" sheetId="1" r:id="rId1"/>
+    <sheet name="Appendix_PCIC-stations" sheetId="3" r:id="rId2"/>
+    <sheet name="Appendix_PCIC-anomalies" sheetId="2" r:id="rId3"/>
+    <sheet name="Appendix_PCIC-departures" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
   <si>
     <t>year</t>
   </si>
@@ -211,6 +214,156 @@
   <si>
     <t>https://services.pacificclimate.org/weather-anomaly-viewer</t>
   </si>
+  <si>
+    <t>Elevation (m a.s.l)</t>
+  </si>
+  <si>
+    <t>Longitude (°N)</t>
+  </si>
+  <si>
+    <t>the 4.5 months prior to the start of the project, it was 1.6 degrees warmer and 38 % drier than normal</t>
+  </si>
+  <si>
+    <t>2018 wet season (October 2018 - April 2019) was 0.5 degrees warmer and 26 % drier than normal</t>
+  </si>
+  <si>
+    <t>2019 dry season (May - Oct) was 0.9 degrees warmer and 1 % wetter than normal</t>
+  </si>
+  <si>
+    <t>2019 wet season was 0.38 degrees warmer and 5 % drier than normal, with one extreme wet anomaly</t>
+  </si>
+  <si>
+    <t>overall, the study period was 0.6 degrees warmer and 10% drier than normal</t>
+  </si>
+  <si>
+    <t>Latitude (°W)</t>
+  </si>
+  <si>
+    <t>2019/2020 wet season</t>
+  </si>
+  <si>
+    <t>2019 dry season</t>
+  </si>
+  <si>
+    <t>2018/2019 wet season</t>
+  </si>
+  <si>
+    <t>Oct. 2018 - May 2019</t>
+  </si>
+  <si>
+    <t>Oct. 2019 - Feb. 2020</t>
+  </si>
+  <si>
+    <t>Sampling season</t>
+  </si>
+  <si>
+    <t>Date range</t>
+  </si>
+  <si>
+    <r>
+      <t>Temperature departure (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C)</t>
+    </r>
+  </si>
+  <si>
+    <t>Precipitation departure (%)</t>
+  </si>
+  <si>
+    <t>Study period</t>
+  </si>
+  <si>
+    <t>Oct. 2018 - Feb. 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average weather departures from normal (relative to 1970 onward) from Bear Creek Reservoir and Shawnigan Lake weather stations </t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <r>
+      <t>Temperature, min. (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">C) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Temperature, max. (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">C) </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation (%) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average monthly weather anomalies from 1970 onward from Bear Creek Reservoir and Shawnigan Lake weather stations </t>
+  </si>
+  <si>
+    <t>June 2019 - Sept. 2019</t>
+  </si>
+  <si>
+    <t>June 2018 - Sept. 2018</t>
+  </si>
+  <si>
+    <t>Dry period before project start</t>
+  </si>
 </sst>
 </file>
 
@@ -219,7 +372,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +399,21 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -331,10 +499,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -378,6 +547,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -387,11 +559,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -405,14 +574,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -727,40 +955,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9424E020-9CD4-43B3-BE85-0A2C7A07B9BC}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="109" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="9" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="9" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="48" t="s">
@@ -789,13 +1017,13 @@
       </c>
       <c r="N2" s="51"/>
       <c r="O2" s="51"/>
-      <c r="P2" s="53" t="s">
+      <c r="P2" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="53"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
+      <c r="Q2" s="47"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="53"/>
       <c r="B3" s="49"/>
       <c r="C3" s="49"/>
       <c r="D3" s="22" t="s">
@@ -844,8 +1072,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="44" t="s">
         <v>32</v>
       </c>
       <c r="B4">
@@ -897,8 +1125,8 @@
       <c r="P4" s="41"/>
       <c r="Q4" s="41"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="45"/>
       <c r="B5">
         <v>2018</v>
       </c>
@@ -948,8 +1176,8 @@
       <c r="P5" s="41"/>
       <c r="Q5" s="41"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="45"/>
       <c r="B6">
         <v>2018</v>
       </c>
@@ -999,8 +1227,8 @@
       <c r="P6" s="41"/>
       <c r="Q6" s="41"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="46"/>
       <c r="B7">
         <v>2018</v>
       </c>
@@ -1059,8 +1287,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="44" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="6">
@@ -1112,8 +1340,8 @@
       <c r="P8" s="41"/>
       <c r="Q8" s="41"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="45"/>
       <c r="B9" s="11">
         <v>2018</v>
       </c>
@@ -1163,8 +1391,8 @@
       <c r="P9" s="41"/>
       <c r="Q9" s="41"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="45"/>
       <c r="B10" s="11">
         <v>2018</v>
       </c>
@@ -1214,8 +1442,8 @@
       <c r="P10" s="41"/>
       <c r="Q10" s="41"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="45"/>
       <c r="B11" s="11">
         <v>2019</v>
       </c>
@@ -1265,8 +1493,8 @@
       <c r="P11" s="41"/>
       <c r="Q11" s="41"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="45"/>
       <c r="B12" s="11">
         <v>2019</v>
       </c>
@@ -1316,8 +1544,8 @@
       <c r="P12" s="41"/>
       <c r="Q12" s="41"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="45"/>
       <c r="B13" s="11">
         <v>2019</v>
       </c>
@@ -1367,8 +1595,8 @@
       <c r="P13" s="41"/>
       <c r="Q13" s="41"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="45"/>
       <c r="B14" s="11">
         <v>2019</v>
       </c>
@@ -1418,8 +1646,8 @@
       <c r="P14" s="41"/>
       <c r="Q14" s="41"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="46"/>
       <c r="B15" s="16">
         <v>2019</v>
       </c>
@@ -1478,8 +1706,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="44" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="11">
@@ -1531,8 +1759,8 @@
       <c r="P16" s="41"/>
       <c r="Q16" s="41"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="45"/>
       <c r="B17" s="11">
         <v>2019</v>
       </c>
@@ -1582,8 +1810,8 @@
       <c r="P17" s="41"/>
       <c r="Q17" s="41"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="45"/>
       <c r="B18" s="11">
         <v>2019</v>
       </c>
@@ -1633,8 +1861,8 @@
       <c r="P18" s="41"/>
       <c r="Q18" s="41"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="46"/>
       <c r="B19" s="11">
         <v>2019</v>
       </c>
@@ -1693,8 +1921,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="44" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="6">
@@ -1746,8 +1974,8 @@
       <c r="P20" s="41"/>
       <c r="Q20" s="41"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="45"/>
       <c r="B21">
         <v>2019</v>
       </c>
@@ -1797,8 +2025,8 @@
       <c r="P21" s="41"/>
       <c r="Q21" s="41"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="45"/>
       <c r="B22">
         <v>2019</v>
       </c>
@@ -1848,8 +2076,8 @@
       <c r="P22" s="41"/>
       <c r="Q22" s="41"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="45"/>
       <c r="B23">
         <v>2020</v>
       </c>
@@ -1899,8 +2127,8 @@
       <c r="P23" s="41"/>
       <c r="Q23" s="41"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="46"/>
       <c r="B24" s="16">
         <v>2020</v>
       </c>
@@ -1959,12 +2187,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="54" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P25" s="30">
+        <f>AVERAGE(F8:F24,I8:I24)</f>
+        <v>0.55514705882352944</v>
+      </c>
+      <c r="Q25" s="42">
+        <f>AVERAGE(L8:L24)</f>
+        <v>-13.352941176470589</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1978,7 +2214,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1995,7 +2231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2011,6 +2247,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="P2:Q2"/>
@@ -2019,14 +2260,620 @@
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="M2:O2"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A25" r:id="rId1" xr:uid="{62E58215-A25A-4369-A432-DE192D79BF4C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDD2BE9-766C-428A-BB5D-DD2486F855D1}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>419</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>48.503333329999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>138</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3">
+        <v>48.647219999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559A4457-C141-4C95-B616-E14291BEA7BF}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="68"/>
+    <col min="2" max="2" width="10.88671875" style="68" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.5546875" style="68" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="68"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+    </row>
+    <row r="2" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="68">
+        <v>2018</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="55">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="D3" s="56">
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="E3" s="57">
+        <v>-31.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="68">
+        <v>2018</v>
+      </c>
+      <c r="B4" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="55">
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="D4" s="56">
+        <v>4.63</v>
+      </c>
+      <c r="E4" s="57">
+        <v>-94.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="68">
+        <v>2018</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="55">
+        <v>1.05</v>
+      </c>
+      <c r="D5" s="56">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E5" s="57">
+        <v>-89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="68">
+        <v>2018</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="55">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D6" s="56">
+        <v>-0.78</v>
+      </c>
+      <c r="E6" s="57">
+        <v>63.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="72">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="58">
+        <v>0.21999999999999997</v>
+      </c>
+      <c r="D7" s="59">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="E7" s="60">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="73">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="61">
+        <v>2.21</v>
+      </c>
+      <c r="D8" s="62">
+        <v>1.415</v>
+      </c>
+      <c r="E8" s="63">
+        <v>-15.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="73">
+        <v>2018</v>
+      </c>
+      <c r="B9" s="73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="61">
+        <v>1.36</v>
+      </c>
+      <c r="D9" s="62">
+        <v>0.85</v>
+      </c>
+      <c r="E9" s="63">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="73">
+        <v>2019</v>
+      </c>
+      <c r="B10" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="61">
+        <v>1.855</v>
+      </c>
+      <c r="D10" s="62">
+        <v>1.5699999999999998</v>
+      </c>
+      <c r="E10" s="63">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="73">
+        <v>2019</v>
+      </c>
+      <c r="B11" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="61">
+        <v>-3.74</v>
+      </c>
+      <c r="D11" s="62">
+        <v>-4.8699999999999992</v>
+      </c>
+      <c r="E11" s="63">
+        <v>-50.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="73">
+        <v>2019</v>
+      </c>
+      <c r="B12" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="61">
+        <v>-2.59</v>
+      </c>
+      <c r="D12" s="62">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="E12" s="63">
+        <v>-85.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="73">
+        <v>2019</v>
+      </c>
+      <c r="B13" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="61">
+        <v>1.0550000000000002</v>
+      </c>
+      <c r="D13" s="62">
+        <v>0.495</v>
+      </c>
+      <c r="E13" s="63">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="74">
+        <v>2019</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="64">
+        <v>2.1150000000000002</v>
+      </c>
+      <c r="D14" s="65">
+        <v>3.8949999999999996</v>
+      </c>
+      <c r="E14" s="66">
+        <v>-68.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="73">
+        <v>2019</v>
+      </c>
+      <c r="B15" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="61">
+        <v>0.87</v>
+      </c>
+      <c r="D15" s="62">
+        <v>1.92</v>
+      </c>
+      <c r="E15" s="63">
+        <v>-75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="73">
+        <v>2019</v>
+      </c>
+      <c r="B16" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="61">
+        <v>1</v>
+      </c>
+      <c r="D16" s="62">
+        <v>5.4999999999999993E-2</v>
+      </c>
+      <c r="E16" s="63">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="73">
+        <v>2019</v>
+      </c>
+      <c r="B17" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="61">
+        <v>1.55</v>
+      </c>
+      <c r="D17" s="62">
+        <v>1.35</v>
+      </c>
+      <c r="E17" s="63">
+        <v>-39.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="73">
+        <v>2019</v>
+      </c>
+      <c r="B18" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="61">
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D18" s="62">
+        <v>-1.25</v>
+      </c>
+      <c r="E18" s="63">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="72">
+        <v>2019</v>
+      </c>
+      <c r="B19" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="58">
+        <v>-1.17</v>
+      </c>
+      <c r="D19" s="59">
+        <v>-0.91</v>
+      </c>
+      <c r="E19" s="60">
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="68">
+        <v>2019</v>
+      </c>
+      <c r="B20" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="55">
+        <v>4.5000000000000012E-2</v>
+      </c>
+      <c r="D20" s="56">
+        <v>1.39</v>
+      </c>
+      <c r="E20" s="57">
+        <v>-64.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="68">
+        <v>2019</v>
+      </c>
+      <c r="B21" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="55">
+        <v>2.2050000000000001</v>
+      </c>
+      <c r="D21" s="56">
+        <v>0.8</v>
+      </c>
+      <c r="E21" s="57">
+        <v>-16.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="68">
+        <v>2020</v>
+      </c>
+      <c r="B22" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="55">
+        <v>1.07</v>
+      </c>
+      <c r="D22" s="56">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="E22" s="57">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="74">
+        <v>2020</v>
+      </c>
+      <c r="B23" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="64">
+        <v>0.36</v>
+      </c>
+      <c r="D23" s="65">
+        <v>0.12</v>
+      </c>
+      <c r="E23" s="66">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="75"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7064BF-C452-48DE-A8C6-B607586E42B4}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="77"/>
+    <col min="2" max="2" width="19.44140625" style="77" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.88671875" style="77" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="77"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="83" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="77" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="79">
+        <v>1.5806249999999999</v>
+      </c>
+      <c r="D3" s="80">
+        <v>-37.9</v>
+      </c>
+      <c r="E3" s="77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="78" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="79">
+        <v>0.47531250000000003</v>
+      </c>
+      <c r="D4" s="80">
+        <v>-26.1875</v>
+      </c>
+      <c r="E4" s="77" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="78" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="79">
+        <v>0.9375</v>
+      </c>
+      <c r="D5" s="80">
+        <v>1.375</v>
+      </c>
+      <c r="E5" s="77" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="84" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="85">
+        <v>0.377</v>
+      </c>
+      <c r="D6" s="87">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="E6" s="77" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="85">
+        <v>0.55514705882352944</v>
+      </c>
+      <c r="D7" s="85">
+        <v>-13.352941176470589</v>
+      </c>
+      <c r="E7" s="77" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates based on Bill's Chapter 2 edits
</commit_message>
<xml_diff>
--- a/R-inputs_UBC-forWater-MSc_HMc/tables/Workbooks/weather_anomaly_PCIC.xlsx
+++ b/R-inputs_UBC-forWater-MSc_HMc/tables/Workbooks/weather_anomaly_PCIC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\2020_Thesis_gitdocs\UBC_MSc_thesis\R-inputs_UBC-forWater-MSc_HMc\tables\Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Documents\UBC_MSc\Thesis_UBC-forWater-MSc_HMc\R_UBC_MSc_thesis\R-inputs_UBC-forWater-MSc_HMc\tables\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{316E0485-2B27-411B-8A0B-09670945CE8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0C7A3843-E647-4E43-80D7-264BF2797021}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7680C772-8F90-439C-BDD5-995D84FBCB52}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7680C772-8F90-439C-BDD5-995D84FBCB52}"/>
   </bookViews>
   <sheets>
     <sheet name="weather_anomaly_PCIC" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
   <si>
     <t>year</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>warmer?</t>
-  </si>
-  <si>
-    <t>wetter?</t>
   </si>
   <si>
     <t>sampling season</t>
@@ -197,18 +194,6 @@
     <t>average anomaly</t>
   </si>
   <si>
-    <t>the 4.5 months prior to the start of the project, it was warmer and 38 % drier than normal</t>
-  </si>
-  <si>
-    <t>2018 wet season (October 2018 - April 2019) was slightly warmer and 26 % drier than normal</t>
-  </si>
-  <si>
-    <t>2019 wet season was warmer and 5 % drier than normal, with one extreme wet anomaly</t>
-  </si>
-  <si>
-    <t>2019 dry season (May - Oct) was warmer and 1 % wetter than normal</t>
-  </si>
-  <si>
     <t>Station name</t>
   </si>
   <si>
@@ -219,18 +204,6 @@
   </si>
   <si>
     <t>Longitude (°N)</t>
-  </si>
-  <si>
-    <t>the 4.5 months prior to the start of the project, it was 1.6 degrees warmer and 38 % drier than normal</t>
-  </si>
-  <si>
-    <t>2018 wet season (October 2018 - April 2019) was 0.5 degrees warmer and 26 % drier than normal</t>
-  </si>
-  <si>
-    <t>2019 dry season (May - Oct) was 0.9 degrees warmer and 1 % wetter than normal</t>
-  </si>
-  <si>
-    <t>2019 wet season was 0.38 degrees warmer and 5 % drier than normal, with one extreme wet anomaly</t>
   </si>
   <si>
     <t>overall, the study period was 0.6 degrees warmer and 10% drier than normal</t>
@@ -364,6 +337,30 @@
   <si>
     <t>Dry period before project start</t>
   </si>
+  <si>
+    <t>wetter? (%)</t>
+  </si>
+  <si>
+    <t>wetter? (mm/month)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018 wet season (October 2018 - April 2019) was slightly warmer and 26 % drier (25.5 mm/month) than normal </t>
+  </si>
+  <si>
+    <t>2019 dry season (May - Oct) was warmer and 1 % wetter (6.4 mm/month) than normal</t>
+  </si>
+  <si>
+    <t>2019 wet season was warmer and 5 % drier (10.2 mm/month) than normal, with one extreme wet anomaly</t>
+  </si>
+  <si>
+    <t>the 4.5 months prior to the start of the project, it was warmer and 38 % drier (14.8 mm/month) than normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precip. (mm/month) </t>
+  </si>
+  <si>
+    <t>Precipitation departure (mm/month)</t>
+  </si>
 </sst>
 </file>
 
@@ -372,7 +369,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,13 +396,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -501,9 +491,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -547,40 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -603,7 +560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -636,6 +593,49 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -955,77 +955,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9424E020-9CD4-43B3-BE85-0A2C7A07B9BC}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="109" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.5546875" customWidth="1"/>
-    <col min="7" max="9" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="9" width="9.85546875" customWidth="1"/>
+    <col min="18" max="18" width="19" customWidth="1"/>
+    <col min="19" max="19" width="61.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="48" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="80" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="51" t="s">
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="50" t="s">
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="51" t="s">
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="47"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="53"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="Q2" s="87"/>
+      <c r="R2" s="87"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="81"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="22" t="s">
         <v>14</v>
       </c>
@@ -1033,7 +1036,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>14</v>
@@ -1066,15 +1069,18 @@
         <v>20</v>
       </c>
       <c r="Q3" s="40" t="s">
-        <v>21</v>
+        <v>65</v>
+      </c>
+      <c r="R3" s="40" t="s">
+        <v>66</v>
       </c>
       <c r="S3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="77" t="s">
+        <v>31</v>
       </c>
       <c r="B4">
         <v>2018</v>
@@ -1125,8 +1131,8 @@
       <c r="P4" s="41"/>
       <c r="Q4" s="41"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="78"/>
       <c r="B5">
         <v>2018</v>
       </c>
@@ -1176,8 +1182,8 @@
       <c r="P5" s="41"/>
       <c r="Q5" s="41"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="45"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="78"/>
       <c r="B6">
         <v>2018</v>
       </c>
@@ -1227,8 +1233,8 @@
       <c r="P6" s="41"/>
       <c r="Q6" s="41"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
+    <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="79"/>
       <c r="B7">
         <v>2018</v>
       </c>
@@ -1283,13 +1289,17 @@
         <f>AVERAGE(L4:L7)</f>
         <v>-37.9</v>
       </c>
-      <c r="S7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
-        <v>31</v>
+      <c r="R7" s="42">
+        <f>AVERAGE(O4:O7)</f>
+        <v>-14.762499999999999</v>
+      </c>
+      <c r="S7" s="88" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="77" t="s">
+        <v>30</v>
       </c>
       <c r="B8" s="6">
         <v>2018</v>
@@ -1339,9 +1349,10 @@
       </c>
       <c r="P8" s="41"/>
       <c r="Q8" s="41"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="45"/>
+      <c r="S8" s="88"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="78"/>
       <c r="B9" s="11">
         <v>2018</v>
       </c>
@@ -1390,9 +1401,10 @@
       </c>
       <c r="P9" s="41"/>
       <c r="Q9" s="41"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
+      <c r="S9" s="88"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="78"/>
       <c r="B10" s="11">
         <v>2018</v>
       </c>
@@ -1441,9 +1453,10 @@
       </c>
       <c r="P10" s="41"/>
       <c r="Q10" s="41"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="45"/>
+      <c r="S10" s="88"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="78"/>
       <c r="B11" s="11">
         <v>2019</v>
       </c>
@@ -1492,9 +1505,10 @@
       </c>
       <c r="P11" s="41"/>
       <c r="Q11" s="41"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="45"/>
+      <c r="S11" s="88"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="78"/>
       <c r="B12" s="11">
         <v>2019</v>
       </c>
@@ -1543,9 +1557,10 @@
       </c>
       <c r="P12" s="41"/>
       <c r="Q12" s="41"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
+      <c r="S12" s="88"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="78"/>
       <c r="B13" s="11">
         <v>2019</v>
       </c>
@@ -1594,9 +1609,10 @@
       </c>
       <c r="P13" s="41"/>
       <c r="Q13" s="41"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="45"/>
+      <c r="S13" s="88"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="78"/>
       <c r="B14" s="11">
         <v>2019</v>
       </c>
@@ -1645,9 +1661,10 @@
       </c>
       <c r="P14" s="41"/>
       <c r="Q14" s="41"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="46"/>
+      <c r="S14" s="88"/>
+    </row>
+    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="79"/>
       <c r="B15" s="16">
         <v>2019</v>
       </c>
@@ -1702,13 +1719,17 @@
         <f>AVERAGE(L8:L15)</f>
         <v>-26.1875</v>
       </c>
-      <c r="S15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="44" t="s">
-        <v>30</v>
+      <c r="R15" s="42">
+        <f>AVERAGE(O8:O15)</f>
+        <v>-25.450000000000003</v>
+      </c>
+      <c r="S15" s="88" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="77" t="s">
+        <v>29</v>
       </c>
       <c r="B16" s="11">
         <v>2019</v>
@@ -1758,9 +1779,10 @@
       </c>
       <c r="P16" s="41"/>
       <c r="Q16" s="41"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="45"/>
+      <c r="S16" s="88"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="78"/>
       <c r="B17" s="11">
         <v>2019</v>
       </c>
@@ -1809,9 +1831,10 @@
       </c>
       <c r="P17" s="41"/>
       <c r="Q17" s="41"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="45"/>
+      <c r="S17" s="88"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="78"/>
       <c r="B18" s="11">
         <v>2019</v>
       </c>
@@ -1860,9 +1883,10 @@
       </c>
       <c r="P18" s="41"/>
       <c r="Q18" s="41"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="46"/>
+      <c r="S18" s="88"/>
+    </row>
+    <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="79"/>
       <c r="B19" s="11">
         <v>2019</v>
       </c>
@@ -1917,13 +1941,17 @@
         <f>AVERAGE(L16:L19)</f>
         <v>1.375</v>
       </c>
-      <c r="S19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="44" t="s">
-        <v>29</v>
+      <c r="R19" s="42">
+        <f>AVERAGE(O16:O19)</f>
+        <v>6.4124999999999979</v>
+      </c>
+      <c r="S19" s="88" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="77" t="s">
+        <v>28</v>
       </c>
       <c r="B20" s="6">
         <v>2019</v>
@@ -1973,9 +2001,10 @@
       </c>
       <c r="P20" s="41"/>
       <c r="Q20" s="41"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="45"/>
+      <c r="S20" s="88"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="78"/>
       <c r="B21">
         <v>2019</v>
       </c>
@@ -2024,9 +2053,10 @@
       </c>
       <c r="P21" s="41"/>
       <c r="Q21" s="41"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="45"/>
+      <c r="S21" s="88"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="78"/>
       <c r="B22">
         <v>2019</v>
       </c>
@@ -2075,9 +2105,10 @@
       </c>
       <c r="P22" s="41"/>
       <c r="Q22" s="41"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="45"/>
+      <c r="S22" s="88"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="78"/>
       <c r="B23">
         <v>2020</v>
       </c>
@@ -2126,9 +2157,10 @@
       </c>
       <c r="P23" s="41"/>
       <c r="Q23" s="41"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="46"/>
+      <c r="S23" s="88"/>
+    </row>
+    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="79"/>
       <c r="B24" s="16">
         <v>2020</v>
       </c>
@@ -2183,13 +2215,17 @@
         <f>AVERAGE(L20:L24)</f>
         <v>-4.5999999999999996</v>
       </c>
-      <c r="S24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="54" t="s">
-        <v>44</v>
+      <c r="R24" s="42">
+        <f>AVERAGE(O20:O24)</f>
+        <v>10.229999999999995</v>
+      </c>
+      <c r="S24" s="88" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="43" t="s">
+        <v>39</v>
       </c>
       <c r="P25" s="30">
         <f>AVERAGE(F8:F24,I8:I24)</f>
@@ -2199,22 +2235,26 @@
         <f>AVERAGE(L8:L24)</f>
         <v>-13.352941176470589</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R25" s="42">
+        <f>AVERAGE(O8:O24)</f>
+        <v>-7.4588235294117657</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" t="s">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2222,7 +2262,7 @@
         <v>419</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27">
         <v>48.503333329999997</v>
@@ -2231,7 +2271,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2239,7 +2279,7 @@
         <v>138</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28">
         <v>48.647219999999997</v>
@@ -2247,19 +2287,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
     <mergeCell ref="A8:A15"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -2278,23 +2318,23 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
       <c r="D1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2302,13 +2342,13 @@
         <v>419</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>48.503333329999997</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2316,7 +2356,7 @@
         <v>138</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>48.647219999999997</v>
@@ -2332,414 +2372,479 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="68"/>
-    <col min="2" max="2" width="10.88671875" style="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.5546875" style="68" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="68"/>
+    <col min="1" max="1" width="8.85546875" style="57"/>
+    <col min="2" max="2" width="10.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.5703125" style="57" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-    </row>
-    <row r="2" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="70" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="70" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="68">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+    </row>
+    <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="89" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="57">
         <v>2018</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55">
+      <c r="C3" s="44">
         <v>0.52500000000000002</v>
       </c>
-      <c r="D3" s="56">
+      <c r="D3" s="45">
         <v>1.4650000000000001</v>
       </c>
-      <c r="E3" s="57">
+      <c r="E3" s="46">
         <v>-31.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="68">
+      <c r="F3" s="61">
+        <v>-36.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="57">
         <v>2018</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="44">
         <v>1.2000000000000002</v>
       </c>
-      <c r="D4" s="56">
+      <c r="D4" s="45">
         <v>4.63</v>
       </c>
-      <c r="E4" s="57">
+      <c r="E4" s="46">
         <v>-94.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="68">
+      <c r="F4" s="62">
+        <v>-33.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="57">
         <v>2018</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="55">
+      <c r="C5" s="44">
         <v>1.05</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="45">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E5" s="57">
+      <c r="E5" s="46">
         <v>-89</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="68">
+      <c r="F5" s="62">
+        <v>-40.200000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="57">
         <v>2018</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="55">
+      <c r="C6" s="44">
         <v>0.45500000000000002</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="45">
         <v>-0.78</v>
       </c>
-      <c r="E6" s="57">
+      <c r="E6" s="46">
         <v>63.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="72">
+      <c r="F6" s="63">
+        <v>50.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="61">
         <v>2018</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="47">
         <v>0.21999999999999997</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="48">
         <v>0.63500000000000001</v>
       </c>
-      <c r="E7" s="60">
+      <c r="E7" s="49">
         <v>-45</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="73">
+      <c r="F7" s="57">
+        <v>-60.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="62">
         <v>2018</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="61">
+      <c r="C8" s="50">
         <v>2.21</v>
       </c>
-      <c r="D8" s="62">
+      <c r="D8" s="51">
         <v>1.415</v>
       </c>
-      <c r="E8" s="63">
+      <c r="E8" s="52">
         <v>-15.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="73">
+      <c r="F8" s="57">
+        <v>-15.450000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="62">
         <v>2018</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="61">
+      <c r="C9" s="50">
         <v>1.36</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="51">
         <v>0.85</v>
       </c>
-      <c r="E9" s="63">
+      <c r="E9" s="52">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="73">
+      <c r="F9" s="57">
+        <v>119.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="62">
         <v>2019</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="61">
+      <c r="C10" s="50">
         <v>1.855</v>
       </c>
-      <c r="D10" s="62">
+      <c r="D10" s="51">
         <v>1.5699999999999998</v>
       </c>
-      <c r="E10" s="63">
+      <c r="E10" s="52">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="73">
+      <c r="F10" s="57">
+        <v>65.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="62">
         <v>2019</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="61">
+      <c r="C11" s="50">
         <v>-3.74</v>
       </c>
-      <c r="D11" s="62">
+      <c r="D11" s="51">
         <v>-4.8699999999999992</v>
       </c>
-      <c r="E11" s="63">
+      <c r="E11" s="52">
         <v>-50.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="73">
+      <c r="F11" s="57">
+        <v>-123.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="62">
         <v>2019</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="61">
+      <c r="C12" s="50">
         <v>-2.59</v>
       </c>
-      <c r="D12" s="62">
+      <c r="D12" s="51">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E12" s="63">
+      <c r="E12" s="52">
         <v>-85.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="73">
+      <c r="F12" s="57">
+        <v>-151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="62">
         <v>2019</v>
       </c>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="61">
+      <c r="C13" s="50">
         <v>1.0550000000000002</v>
       </c>
-      <c r="D13" s="62">
+      <c r="D13" s="51">
         <v>0.495</v>
       </c>
-      <c r="E13" s="63">
+      <c r="E13" s="52">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="74">
+      <c r="F13" s="57">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="63">
         <v>2019</v>
       </c>
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="64">
+      <c r="C14" s="53">
         <v>2.1150000000000002</v>
       </c>
-      <c r="D14" s="65">
+      <c r="D14" s="54">
         <v>3.8949999999999996</v>
       </c>
-      <c r="E14" s="66">
+      <c r="E14" s="55">
         <v>-68.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="73">
+      <c r="F14" s="63">
+        <v>-51.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="62">
         <v>2019</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="61">
+      <c r="C15" s="50">
         <v>0.87</v>
       </c>
-      <c r="D15" s="62">
+      <c r="D15" s="51">
         <v>1.92</v>
       </c>
-      <c r="E15" s="63">
+      <c r="E15" s="52">
         <v>-75</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="73">
+      <c r="F15" s="57">
+        <v>-29.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="62">
         <v>2019</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="61">
+      <c r="C16" s="50">
         <v>1</v>
       </c>
-      <c r="D16" s="62">
+      <c r="D16" s="51">
         <v>5.4999999999999993E-2</v>
       </c>
-      <c r="E16" s="63">
+      <c r="E16" s="52">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="73">
+      <c r="F16" s="57">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="62">
         <v>2019</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="61">
+      <c r="C17" s="50">
         <v>1.55</v>
       </c>
-      <c r="D17" s="62">
+      <c r="D17" s="51">
         <v>1.35</v>
       </c>
-      <c r="E17" s="63">
+      <c r="E17" s="52">
         <v>-39.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="73">
+      <c r="F17" s="57">
+        <v>-15.45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="62">
         <v>2019</v>
       </c>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="61">
+      <c r="C18" s="50">
         <v>2.0049999999999999</v>
       </c>
-      <c r="D18" s="62">
+      <c r="D18" s="51">
         <v>-1.25</v>
       </c>
-      <c r="E18" s="63">
+      <c r="E18" s="52">
         <v>108</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="72">
+      <c r="F18" s="63">
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="61">
         <v>2019</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="58">
+      <c r="C19" s="47">
         <v>-1.17</v>
       </c>
-      <c r="D19" s="59">
+      <c r="D19" s="48">
         <v>-0.91</v>
       </c>
-      <c r="E19" s="60">
+      <c r="E19" s="49">
         <v>-18</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="68">
+      <c r="F19" s="57">
+        <v>-18.399999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="57">
         <v>2019</v>
       </c>
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="55">
+      <c r="C20" s="44">
         <v>4.5000000000000012E-2</v>
       </c>
-      <c r="D20" s="56">
+      <c r="D20" s="45">
         <v>1.39</v>
       </c>
-      <c r="E20" s="57">
+      <c r="E20" s="46">
         <v>-64.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="68">
+      <c r="F20" s="57">
+        <v>-212.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="57">
         <v>2019</v>
       </c>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="55">
+      <c r="C21" s="44">
         <v>2.2050000000000001</v>
       </c>
-      <c r="D21" s="56">
+      <c r="D21" s="45">
         <v>0.8</v>
       </c>
-      <c r="E21" s="57">
+      <c r="E21" s="46">
         <v>-16.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="68">
+      <c r="F21" s="57">
+        <v>-32.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="57">
         <v>2020</v>
       </c>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="55">
+      <c r="C22" s="44">
         <v>1.07</v>
       </c>
-      <c r="D22" s="56">
+      <c r="D22" s="45">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="E22" s="57">
+      <c r="E22" s="46">
         <v>136</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="74">
+      <c r="F22" s="57">
+        <v>407.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="63">
         <v>2020</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="64">
+      <c r="C23" s="53">
         <v>0.36</v>
       </c>
-      <c r="D23" s="65">
+      <c r="D23" s="54">
         <v>0.12</v>
       </c>
-      <c r="E23" s="66">
+      <c r="E23" s="55">
         <v>-60</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="75"/>
+      <c r="F23" s="63">
+        <v>-93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2749,128 +2854,146 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7064BF-C452-48DE-A8C6-B607586E42B4}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="77"/>
-    <col min="2" max="2" width="19.44140625" style="77" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.88671875" style="77" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="77"/>
+    <col min="1" max="1" width="8.85546875" style="66"/>
+    <col min="2" max="2" width="19.42578125" style="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.85546875" style="66" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="66"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-    </row>
-    <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="82" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="82" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="83" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="77" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="79">
+      <c r="B3" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="68">
         <v>1.5806249999999999</v>
       </c>
-      <c r="D3" s="80">
+      <c r="D3" s="69">
         <v>-37.9</v>
       </c>
-      <c r="E3" s="77" t="s">
+      <c r="E3" s="90">
+        <v>-14.762499999999999</v>
+      </c>
+      <c r="F3" s="66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="67" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="78" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="79">
+      <c r="C4" s="68">
         <v>0.47531250000000003</v>
       </c>
-      <c r="D4" s="80">
+      <c r="D4" s="69">
         <v>-26.1875</v>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="E4" s="90">
+        <v>-25.450000000000003</v>
+      </c>
+      <c r="F4" s="66" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="68">
+        <v>0.9375</v>
+      </c>
+      <c r="D5" s="69">
+        <v>1.375</v>
+      </c>
+      <c r="E5" s="90">
+        <v>6.4124999999999979</v>
+      </c>
+      <c r="F5" s="66" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="75" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="78" t="s">
+      <c r="C6" s="74">
+        <v>0.377</v>
+      </c>
+      <c r="D6" s="76">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="E6" s="91">
+        <v>10.229999999999995</v>
+      </c>
+      <c r="F6" s="66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="79">
-        <v>0.9375</v>
-      </c>
-      <c r="D5" s="80">
-        <v>1.375</v>
-      </c>
-      <c r="E5" s="77" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="86" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="85">
-        <v>0.377</v>
-      </c>
-      <c r="D6" s="87">
-        <v>-4.5999999999999996</v>
-      </c>
-      <c r="E6" s="77" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="84" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="84" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="85">
+      <c r="C7" s="74">
         <v>0.55514705882352944</v>
       </c>
-      <c r="D7" s="85">
+      <c r="D7" s="74">
         <v>-13.352941176470589</v>
       </c>
-      <c r="E7" s="77" t="s">
-        <v>51</v>
+      <c r="E7" s="91">
+        <v>-7.4588235294117657</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>